<commit_message>
added broken image verification code
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/feedFromExcel.xlsx
+++ b/resources/ExcelsheetData/feedFromExcel.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15210" windowHeight="2310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:O6"/>
 </workbook>
 </file>
 
@@ -405,7 +406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -456,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>